<commit_message>
update setup log, datatest
</commit_message>
<xml_diff>
--- a/src/test/java/seatech/uiTest/ibv/testcase/hubspot_scenarios.xlsx
+++ b/src/test/java/seatech/uiTest/ibv/testcase/hubspot_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\automation-test-master\src\test\java\seatech\uiTest\ibv\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F33775-6F06-4302-A532-B44BECBB0DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB07112B-BE34-4787-B985-9C50F6162EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1444,7 @@
         <v>4</v>
       </c>
       <c r="G24" s="33">
-        <v>123654</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update setup allure report
</commit_message>
<xml_diff>
--- a/src/test/java/seatech/uiTest/ibv/testcase/hubspot_scenarios.xlsx
+++ b/src/test/java/seatech/uiTest/ibv/testcase/hubspot_scenarios.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\automation-test-master\src\test\java\seatech\uiTest\ibv\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB07112B-BE34-4787-B985-9C50F6162EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D01CAD8-FAD1-471D-B4AB-461995060FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ck trong" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="signup" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="signup" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="97">
   <si>
     <t>action</t>
   </si>
@@ -941,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,8 +1444,8 @@
       <c r="F24" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="33">
-        <v>123456</v>
+      <c r="G24" s="33" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -2101,6 +2102,971 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DEF451-0653-409A-80AA-B1EEE4FA6368}">
+  <dimension ref="A1:G48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" s="34" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B16" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B22" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B24" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="20">
+        <v>12345</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B29" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="B30" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="34" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B31" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B35" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B37" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B39" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B40" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="20">
+        <v>20121</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B41" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B42" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B43" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B44" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="B45" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B46" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="D48" s="22"/>
+      <c r="F48" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC761A6E-E9FF-4ACE-8C2E-C1DB4EA8844F}">
   <dimension ref="A1:A17"/>
   <sheetViews>
@@ -2132,7 +3098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>

</xml_diff>